<commit_message>
2022-10-25 - Correct FEC_IDs
</commit_message>
<xml_diff>
--- a/Data/2022 Candidates File/candidate_list.xlsx
+++ b/Data/2022 Candidates File/candidate_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onest\OneDrive\Desktop\2022 Election Model\Data\2022 Candidates File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10246AD-2F75-4BEF-AEEB-4B3D6041A163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6244132-4250-43D5-9DDF-733D30BC5003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{A68E779F-2E40-4AF2-8B1B-69C7B61E945F}"/>
   </bookViews>
@@ -4979,9 +4979,6 @@
     <t>H2CA31125</t>
   </si>
   <si>
-    <t>H0CA08226</t>
-  </si>
-  <si>
     <t>H2CA34079</t>
   </si>
   <si>
@@ -6188,9 +6185,6 @@
     <t>H4CA24175</t>
   </si>
   <si>
-    <t>H2CA22157</t>
-  </si>
-  <si>
     <t>H2CA47188</t>
   </si>
   <si>
@@ -6270,6 +6264,12 @@
   </si>
   <si>
     <t>H0TX07170</t>
+  </si>
+  <si>
+    <t>H2CA39078</t>
+  </si>
+  <si>
+    <t>H8CA34266</t>
   </si>
 </sst>
 </file>
@@ -6624,8 +6624,8 @@
   <dimension ref="A1:H842"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A815" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D842" sqref="D842"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6885,13 +6885,13 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -7275,7 +7275,7 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="E25" t="s">
         <v>58</v>
@@ -7535,7 +7535,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="E35" t="s">
         <v>78</v>
@@ -7587,7 +7587,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E37" t="s">
         <v>82</v>
@@ -7639,7 +7639,7 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E39" t="s">
         <v>86</v>
@@ -8237,7 +8237,7 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="E62" t="s">
         <v>126</v>
@@ -8341,7 +8341,7 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E66" t="s">
         <v>133</v>
@@ -8861,7 +8861,7 @@
         <v>24</v>
       </c>
       <c r="D86" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="E86" t="s">
         <v>167</v>
@@ -8991,7 +8991,7 @@
         <v>27</v>
       </c>
       <c r="D91" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="E91" t="s">
         <v>17</v>
@@ -9121,7 +9121,7 @@
         <v>29</v>
       </c>
       <c r="D96" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="E96" t="s">
         <v>184</v>
@@ -9173,7 +9173,7 @@
         <v>30</v>
       </c>
       <c r="D98" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="E98" t="s">
         <v>187</v>
@@ -9225,7 +9225,7 @@
         <v>31</v>
       </c>
       <c r="D100" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="E100" t="s">
         <v>191</v>
@@ -9277,7 +9277,7 @@
         <v>32</v>
       </c>
       <c r="D102" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="E102" t="s">
         <v>194</v>
@@ -9329,10 +9329,10 @@
         <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="E104" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="F104" t="s">
         <v>238</v>
@@ -9355,7 +9355,7 @@
         <v>34</v>
       </c>
       <c r="D105" t="s">
-        <v>1648</v>
+        <v>2078</v>
       </c>
       <c r="E105" t="s">
         <v>149</v>
@@ -9381,7 +9381,7 @@
         <v>34</v>
       </c>
       <c r="D106" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="E106" t="s">
         <v>40</v>
@@ -9485,7 +9485,7 @@
         <v>36</v>
       </c>
       <c r="D110" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="E110" t="s">
         <v>204</v>
@@ -9563,7 +9563,7 @@
         <v>38</v>
       </c>
       <c r="D113" t="s">
-        <v>2051</v>
+        <v>2077</v>
       </c>
       <c r="E113" t="s">
         <v>210</v>
@@ -9589,7 +9589,7 @@
         <v>38</v>
       </c>
       <c r="D114" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="E114" t="s">
         <v>131</v>
@@ -9667,7 +9667,7 @@
         <v>40</v>
       </c>
       <c r="D117" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="E117" t="s">
         <v>215</v>
@@ -9693,7 +9693,7 @@
         <v>40</v>
       </c>
       <c r="D118" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="E118" t="s">
         <v>216</v>
@@ -9771,7 +9771,7 @@
         <v>42</v>
       </c>
       <c r="D121" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="E121" t="s">
         <v>21</v>
@@ -9901,7 +9901,7 @@
         <v>44</v>
       </c>
       <c r="D126" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="E126" t="s">
         <v>70</v>
@@ -10031,7 +10031,7 @@
         <v>47</v>
       </c>
       <c r="D131" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="E131" t="s">
         <v>237</v>
@@ -10109,7 +10109,7 @@
         <v>48</v>
       </c>
       <c r="D134" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="E134" t="s">
         <v>126</v>
@@ -10161,7 +10161,7 @@
         <v>49</v>
       </c>
       <c r="D136" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="E136" t="s">
         <v>170</v>
@@ -10239,7 +10239,7 @@
         <v>51</v>
       </c>
       <c r="D139" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="E139" t="s">
         <v>249</v>
@@ -10291,7 +10291,7 @@
         <v>52</v>
       </c>
       <c r="D141" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="E141" t="s">
         <v>60</v>
@@ -10343,7 +10343,7 @@
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="E143" t="s">
         <v>256</v>
@@ -10369,7 +10369,7 @@
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="E144" t="s">
         <v>258</v>
@@ -10395,7 +10395,7 @@
         <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="E145" t="s">
         <v>204</v>
@@ -10499,7 +10499,7 @@
         <v>4</v>
       </c>
       <c r="D149" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="E149" t="s">
         <v>218</v>
@@ -10525,7 +10525,7 @@
         <v>4</v>
       </c>
       <c r="D150" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="E150" t="s">
         <v>265</v>
@@ -10551,7 +10551,7 @@
         <v>5</v>
       </c>
       <c r="D151" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="E151" t="s">
         <v>89</v>
@@ -10577,7 +10577,7 @@
         <v>5</v>
       </c>
       <c r="D152" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="E152" t="s">
         <v>40</v>
@@ -10629,7 +10629,7 @@
         <v>6</v>
       </c>
       <c r="D154" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="E154" t="s">
         <v>80</v>
@@ -10655,7 +10655,7 @@
         <v>7</v>
       </c>
       <c r="D155" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="E155" t="s">
         <v>271</v>
@@ -10759,7 +10759,7 @@
         <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="E159" t="s">
         <v>86</v>
@@ -10785,7 +10785,7 @@
         <v>1</v>
       </c>
       <c r="D160" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="E160" t="s">
         <v>280</v>
@@ -10811,7 +10811,7 @@
         <v>2</v>
       </c>
       <c r="D161" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="E161" t="s">
         <v>204</v>
@@ -10863,7 +10863,7 @@
         <v>3</v>
       </c>
       <c r="D163" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="E163" t="s">
         <v>284</v>
@@ -10941,7 +10941,7 @@
         <v>4</v>
       </c>
       <c r="D166" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="E166" t="s">
         <v>289</v>
@@ -10993,7 +10993,7 @@
         <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="E168" t="s">
         <v>293</v>
@@ -11123,7 +11123,7 @@
         <v>2</v>
       </c>
       <c r="D173" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="E173" t="s">
         <v>302</v>
@@ -11149,7 +11149,7 @@
         <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="E174" t="s">
         <v>304</v>
@@ -11201,7 +11201,7 @@
         <v>3</v>
       </c>
       <c r="D176" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="E176" t="s">
         <v>308</v>
@@ -11227,7 +11227,7 @@
         <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E177" t="s">
         <v>310</v>
@@ -11253,7 +11253,7 @@
         <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="E178" t="s">
         <v>312</v>
@@ -11331,7 +11331,7 @@
         <v>7</v>
       </c>
       <c r="D181" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="E181" t="s">
         <v>316</v>
@@ -11357,7 +11357,7 @@
         <v>7</v>
       </c>
       <c r="D182" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="E182" t="s">
         <v>318</v>
@@ -11409,7 +11409,7 @@
         <v>8</v>
       </c>
       <c r="D184" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="E184" t="s">
         <v>322</v>
@@ -11487,7 +11487,7 @@
         <v>10</v>
       </c>
       <c r="D187" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="E187" t="s">
         <v>327</v>
@@ -11513,7 +11513,7 @@
         <v>10</v>
       </c>
       <c r="D188" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="E188" t="s">
         <v>329</v>
@@ -11591,7 +11591,7 @@
         <v>12</v>
       </c>
       <c r="D191" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="E191" t="s">
         <v>334</v>
@@ -11617,7 +11617,7 @@
         <v>12</v>
       </c>
       <c r="D192" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="E192" t="s">
         <v>336</v>
@@ -11773,7 +11773,7 @@
         <v>15</v>
       </c>
       <c r="D198" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="E198" t="s">
         <v>345</v>
@@ -11799,7 +11799,7 @@
         <v>16</v>
       </c>
       <c r="D199" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="E199" t="s">
         <v>346</v>
@@ -11877,7 +11877,7 @@
         <v>17</v>
       </c>
       <c r="D202" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="E202" t="s">
         <v>350</v>
@@ -11903,7 +11903,7 @@
         <v>18</v>
       </c>
       <c r="D203" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="E203" t="s">
         <v>239</v>
@@ -11955,7 +11955,7 @@
         <v>19</v>
       </c>
       <c r="D205" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="E205" t="s">
         <v>356</v>
@@ -12007,7 +12007,7 @@
         <v>20</v>
       </c>
       <c r="D207" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="E207" t="s">
         <v>360</v>
@@ -12059,7 +12059,7 @@
         <v>21</v>
       </c>
       <c r="D209" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="E209" t="s">
         <v>363</v>
@@ -12085,7 +12085,7 @@
         <v>22</v>
       </c>
       <c r="D210" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="E210" t="s">
         <v>365</v>
@@ -12111,7 +12111,7 @@
         <v>22</v>
       </c>
       <c r="D211" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="E211" t="s">
         <v>367</v>
@@ -12137,13 +12137,13 @@
         <v>23</v>
       </c>
       <c r="D212" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E212" t="s">
         <v>93</v>
       </c>
       <c r="F212" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="G212">
         <v>0</v>
@@ -12189,7 +12189,7 @@
         <v>24</v>
       </c>
       <c r="D214" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="E214" t="s">
         <v>370</v>
@@ -12267,7 +12267,7 @@
         <v>25</v>
       </c>
       <c r="D217" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="E217" t="s">
         <v>374</v>
@@ -12319,7 +12319,7 @@
         <v>26</v>
       </c>
       <c r="D219" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="E219" t="s">
         <v>378</v>
@@ -12345,7 +12345,7 @@
         <v>27</v>
       </c>
       <c r="D220" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="E220" t="s">
         <v>380</v>
@@ -12449,7 +12449,7 @@
         <v>1</v>
       </c>
       <c r="D224" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="E224" t="s">
         <v>388</v>
@@ -12475,7 +12475,7 @@
         <v>1</v>
       </c>
       <c r="D225" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="E225" t="s">
         <v>390</v>
@@ -12501,7 +12501,7 @@
         <v>2</v>
       </c>
       <c r="D226" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E226" t="s">
         <v>392</v>
@@ -12527,7 +12527,7 @@
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="E227" t="s">
         <v>394</v>
@@ -12553,7 +12553,7 @@
         <v>3</v>
       </c>
       <c r="D228" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="E228" t="s">
         <v>396</v>
@@ -12579,7 +12579,7 @@
         <v>3</v>
       </c>
       <c r="D229" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="E229" t="s">
         <v>398</v>
@@ -12605,7 +12605,7 @@
         <v>4</v>
       </c>
       <c r="D230" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="E230" t="s">
         <v>400</v>
@@ -12631,7 +12631,7 @@
         <v>4</v>
       </c>
       <c r="D231" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="E231" t="s">
         <v>402</v>
@@ -12657,7 +12657,7 @@
         <v>5</v>
       </c>
       <c r="D232" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="E232" t="s">
         <v>404</v>
@@ -12683,7 +12683,7 @@
         <v>5</v>
       </c>
       <c r="D233" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="E233" t="s">
         <v>406</v>
@@ -12709,7 +12709,7 @@
         <v>6</v>
       </c>
       <c r="D234" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="E234" t="s">
         <v>408</v>
@@ -12735,7 +12735,7 @@
         <v>6</v>
       </c>
       <c r="D235" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="E235" t="s">
         <v>409</v>
@@ -12761,7 +12761,7 @@
         <v>7</v>
       </c>
       <c r="D236" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="E236" t="s">
         <v>411</v>
@@ -12787,7 +12787,7 @@
         <v>7</v>
       </c>
       <c r="D237" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="E237" t="s">
         <v>119</v>
@@ -12813,7 +12813,7 @@
         <v>8</v>
       </c>
       <c r="D238" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="E238" t="s">
         <v>414</v>
@@ -12839,7 +12839,7 @@
         <v>8</v>
       </c>
       <c r="D239" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="E239" t="s">
         <v>415</v>
@@ -12891,7 +12891,7 @@
         <v>9</v>
       </c>
       <c r="D241" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="E241" t="s">
         <v>157</v>
@@ -12943,7 +12943,7 @@
         <v>10</v>
       </c>
       <c r="D243" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="E243" t="s">
         <v>17</v>
@@ -12995,7 +12995,7 @@
         <v>11</v>
       </c>
       <c r="D245" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="E245" t="s">
         <v>423</v>
@@ -13021,7 +13021,7 @@
         <v>12</v>
       </c>
       <c r="D246" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="E246" t="s">
         <v>23</v>
@@ -13047,7 +13047,7 @@
         <v>12</v>
       </c>
       <c r="D247" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="E247" t="s">
         <v>425</v>
@@ -13073,7 +13073,7 @@
         <v>13</v>
       </c>
       <c r="D248" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="E248" t="s">
         <v>40</v>
@@ -13125,10 +13125,10 @@
         <v>14</v>
       </c>
       <c r="D250" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="E250" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="F250" t="s">
         <v>427</v>
@@ -13177,7 +13177,7 @@
         <v>1</v>
       </c>
       <c r="D252" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="E252" t="s">
         <v>431</v>
@@ -13229,7 +13229,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="E254" t="s">
         <v>435</v>
@@ -13281,7 +13281,7 @@
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="E256" t="s">
         <v>440</v>
@@ -13307,7 +13307,7 @@
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="E257" t="s">
         <v>442</v>
@@ -13359,7 +13359,7 @@
         <v>2</v>
       </c>
       <c r="D259" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="E259" t="s">
         <v>445</v>
@@ -13411,7 +13411,7 @@
         <v>1</v>
       </c>
       <c r="D261" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="E261" t="s">
         <v>131</v>
@@ -13463,7 +13463,7 @@
         <v>2</v>
       </c>
       <c r="D263" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="E263" t="s">
         <v>451</v>
@@ -13567,7 +13567,7 @@
         <v>4</v>
       </c>
       <c r="D267" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="E267" t="s">
         <v>341</v>
@@ -13619,7 +13619,7 @@
         <v>5</v>
       </c>
       <c r="D269" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
       <c r="E269" t="s">
         <v>46</v>
@@ -13697,7 +13697,7 @@
         <v>7</v>
       </c>
       <c r="D272" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="E272" t="s">
         <v>463</v>
@@ -13723,7 +13723,7 @@
         <v>8</v>
       </c>
       <c r="D273" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="E273" t="s">
         <v>465</v>
@@ -13749,7 +13749,7 @@
         <v>8</v>
       </c>
       <c r="D274" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E274" t="s">
         <v>394</v>
@@ -13775,7 +13775,7 @@
         <v>9</v>
       </c>
       <c r="D275" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="E275" t="s">
         <v>208</v>
@@ -13801,7 +13801,7 @@
         <v>9</v>
       </c>
       <c r="D276" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="E276" t="s">
         <v>91</v>
@@ -13827,7 +13827,7 @@
         <v>10</v>
       </c>
       <c r="D277" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="E277" t="s">
         <v>167</v>
@@ -13879,7 +13879,7 @@
         <v>11</v>
       </c>
       <c r="D279" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="E279" t="s">
         <v>320</v>
@@ -13905,13 +13905,13 @@
         <v>11</v>
       </c>
       <c r="D280" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="E280" t="s">
         <v>472</v>
       </c>
       <c r="F280" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="G280">
         <v>0</v>
@@ -13931,7 +13931,7 @@
         <v>12</v>
       </c>
       <c r="D281" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="E281" t="s">
         <v>17</v>
@@ -13957,7 +13957,7 @@
         <v>12</v>
       </c>
       <c r="D282" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="E282" t="s">
         <v>474</v>
@@ -14087,7 +14087,7 @@
         <v>15</v>
       </c>
       <c r="D287" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="E287" t="s">
         <v>35</v>
@@ -14113,7 +14113,7 @@
         <v>15</v>
       </c>
       <c r="D288" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="E288" t="s">
         <v>70</v>
@@ -14139,7 +14139,7 @@
         <v>16</v>
       </c>
       <c r="D289" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="E289" t="s">
         <v>484</v>
@@ -14217,7 +14217,7 @@
         <v>17</v>
       </c>
       <c r="D292" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="E292" t="s">
         <v>489</v>
@@ -14243,7 +14243,7 @@
         <v>1</v>
       </c>
       <c r="D293" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="E293" t="s">
         <v>492</v>
@@ -14295,7 +14295,7 @@
         <v>2</v>
       </c>
       <c r="D295" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="E295" t="s">
         <v>70</v>
@@ -14347,7 +14347,7 @@
         <v>3</v>
       </c>
       <c r="D297" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="E297" t="s">
         <v>155</v>
@@ -14399,7 +14399,7 @@
         <v>4</v>
       </c>
       <c r="D299" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="E299" t="s">
         <v>155</v>
@@ -14425,7 +14425,7 @@
         <v>4</v>
       </c>
       <c r="D300" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="E300" t="s">
         <v>500</v>
@@ -14503,7 +14503,7 @@
         <v>6</v>
       </c>
       <c r="D303" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="E303" t="s">
         <v>54</v>
@@ -14607,7 +14607,7 @@
         <v>8</v>
       </c>
       <c r="D307" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="E307" t="s">
         <v>280</v>
@@ -14659,7 +14659,7 @@
         <v>9</v>
       </c>
       <c r="D309" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="E309" t="s">
         <v>515</v>
@@ -14711,7 +14711,7 @@
         <v>1</v>
       </c>
       <c r="D311" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="E311" t="s">
         <v>520</v>
@@ -14763,7 +14763,7 @@
         <v>2</v>
       </c>
       <c r="D313" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="E313" t="s">
         <v>524</v>
@@ -14789,7 +14789,7 @@
         <v>2</v>
       </c>
       <c r="D314" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="E314" t="s">
         <v>425</v>
@@ -14867,7 +14867,7 @@
         <v>4</v>
       </c>
       <c r="D317" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="E317" t="s">
         <v>530</v>
@@ -14893,7 +14893,7 @@
         <v>4</v>
       </c>
       <c r="D318" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="E318" t="s">
         <v>532</v>
@@ -14919,7 +14919,7 @@
         <v>1</v>
       </c>
       <c r="D319" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="E319" t="s">
         <v>535</v>
@@ -14945,7 +14945,7 @@
         <v>1</v>
       </c>
       <c r="D320" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="E320" t="s">
         <v>341</v>
@@ -14971,7 +14971,7 @@
         <v>2</v>
       </c>
       <c r="D321" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="E321" t="s">
         <v>538</v>
@@ -15101,7 +15101,7 @@
         <v>4</v>
       </c>
       <c r="D326" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="E326" t="s">
         <v>408</v>
@@ -15127,7 +15127,7 @@
         <v>1</v>
       </c>
       <c r="D327" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="E327" t="s">
         <v>341</v>
@@ -15153,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="D328" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E328" t="s">
         <v>149</v>
@@ -15179,7 +15179,7 @@
         <v>2</v>
       </c>
       <c r="D329" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="E329" t="s">
         <v>551</v>
@@ -15257,7 +15257,7 @@
         <v>3</v>
       </c>
       <c r="D332" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="E332" t="s">
         <v>556</v>
@@ -15283,7 +15283,7 @@
         <v>4</v>
       </c>
       <c r="D333" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E333" t="s">
         <v>451</v>
@@ -15335,7 +15335,7 @@
         <v>5</v>
       </c>
       <c r="D335" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="E335" t="s">
         <v>559</v>
@@ -15387,7 +15387,7 @@
         <v>6</v>
       </c>
       <c r="D337" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="E337" t="s">
         <v>56</v>
@@ -15413,7 +15413,7 @@
         <v>6</v>
       </c>
       <c r="D338" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="E338" t="s">
         <v>563</v>
@@ -15439,7 +15439,7 @@
         <v>1</v>
       </c>
       <c r="D339" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="E339" t="s">
         <v>80</v>
@@ -15465,7 +15465,7 @@
         <v>1</v>
       </c>
       <c r="D340" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="E340" t="s">
         <v>237</v>
@@ -15491,7 +15491,7 @@
         <v>2</v>
       </c>
       <c r="D341" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="E341" t="s">
         <v>567</v>
@@ -15517,7 +15517,7 @@
         <v>2</v>
       </c>
       <c r="D342" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="E342" t="s">
         <v>367</v>
@@ -15543,7 +15543,7 @@
         <v>3</v>
       </c>
       <c r="D343" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="E343" t="s">
         <v>569</v>
@@ -15569,13 +15569,13 @@
         <v>3</v>
       </c>
       <c r="D344" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="E344" t="s">
+        <v>1971</v>
+      </c>
+      <c r="F344" t="s">
         <v>1972</v>
-      </c>
-      <c r="F344" t="s">
-        <v>1973</v>
       </c>
       <c r="G344">
         <v>0</v>
@@ -15595,7 +15595,7 @@
         <v>4</v>
       </c>
       <c r="D345" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="E345" t="s">
         <v>17</v>
@@ -15647,13 +15647,13 @@
         <v>5</v>
       </c>
       <c r="D347" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="E347" t="s">
         <v>388</v>
       </c>
       <c r="F347" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="G347">
         <v>0</v>
@@ -15699,7 +15699,7 @@
         <v>1</v>
       </c>
       <c r="D349" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E349" t="s">
         <v>575</v>
@@ -15725,7 +15725,7 @@
         <v>1</v>
       </c>
       <c r="D350" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E350" t="s">
         <v>431</v>
@@ -15803,7 +15803,7 @@
         <v>1</v>
       </c>
       <c r="D353" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="E353" t="s">
         <v>417</v>
@@ -15829,7 +15829,7 @@
         <v>1</v>
       </c>
       <c r="D354" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="E354" t="s">
         <v>582</v>
@@ -15855,7 +15855,7 @@
         <v>2</v>
       </c>
       <c r="D355" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="E355" t="s">
         <v>584</v>
@@ -15907,7 +15907,7 @@
         <v>3</v>
       </c>
       <c r="D357" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="E357" t="s">
         <v>86</v>
@@ -15985,7 +15985,7 @@
         <v>4</v>
       </c>
       <c r="D360" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="E360" t="s">
         <v>48</v>
@@ -16037,7 +16037,7 @@
         <v>5</v>
       </c>
       <c r="D362" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="E362" t="s">
         <v>394</v>
@@ -16089,7 +16089,7 @@
         <v>6</v>
       </c>
       <c r="D364" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="E364" t="s">
         <v>597</v>
@@ -16141,7 +16141,7 @@
         <v>7</v>
       </c>
       <c r="D366" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="E366" t="s">
         <v>239</v>
@@ -16193,7 +16193,7 @@
         <v>8</v>
       </c>
       <c r="D368" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="E368" t="s">
         <v>604</v>
@@ -16219,7 +16219,7 @@
         <v>1</v>
       </c>
       <c r="D369" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="E369" t="s">
         <v>607</v>
@@ -16245,7 +16245,7 @@
         <v>1</v>
       </c>
       <c r="D370" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="E370" t="s">
         <v>608</v>
@@ -16271,7 +16271,7 @@
         <v>2</v>
       </c>
       <c r="D371" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="E371" t="s">
         <v>155</v>
@@ -16297,7 +16297,7 @@
         <v>2</v>
       </c>
       <c r="D372" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="E372" t="s">
         <v>48</v>
@@ -16479,7 +16479,7 @@
         <v>6</v>
       </c>
       <c r="D379" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E379" t="s">
         <v>21</v>
@@ -16531,7 +16531,7 @@
         <v>7</v>
       </c>
       <c r="D381" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="E381" t="s">
         <v>625</v>
@@ -16583,7 +16583,7 @@
         <v>8</v>
       </c>
       <c r="D383" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E383" t="s">
         <v>21</v>
@@ -16609,7 +16609,7 @@
         <v>9</v>
       </c>
       <c r="D384" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="E384" t="s">
         <v>320</v>
@@ -16661,7 +16661,7 @@
         <v>1</v>
       </c>
       <c r="D386" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="E386" t="s">
         <v>631</v>
@@ -16687,7 +16687,7 @@
         <v>1</v>
       </c>
       <c r="D387" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="E387" t="s">
         <v>408</v>
@@ -16713,7 +16713,7 @@
         <v>2</v>
       </c>
       <c r="D388" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="E388" t="s">
         <v>86</v>
@@ -16739,7 +16739,7 @@
         <v>2</v>
       </c>
       <c r="D389" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="E389" t="s">
         <v>9</v>
@@ -16817,7 +16817,7 @@
         <v>4</v>
       </c>
       <c r="D392" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="E392" t="s">
         <v>320</v>
@@ -16869,7 +16869,7 @@
         <v>5</v>
       </c>
       <c r="D394" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="E394" t="s">
         <v>641</v>
@@ -16895,7 +16895,7 @@
         <v>5</v>
       </c>
       <c r="D395" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E395" t="s">
         <v>643</v>
@@ -16999,7 +16999,7 @@
         <v>7</v>
       </c>
       <c r="D399" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="E399" t="s">
         <v>46</v>
@@ -17025,7 +17025,7 @@
         <v>8</v>
       </c>
       <c r="D400" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="E400" t="s">
         <v>367</v>
@@ -17103,13 +17103,13 @@
         <v>9</v>
       </c>
       <c r="D403" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="E403" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F403" t="s">
         <v>1980</v>
-      </c>
-      <c r="F403" t="s">
-        <v>1981</v>
       </c>
       <c r="G403">
         <v>0</v>
@@ -17181,13 +17181,13 @@
         <v>11</v>
       </c>
       <c r="D406" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="E406" t="s">
         <v>654</v>
       </c>
       <c r="F406" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G406">
         <v>1</v>
@@ -17311,7 +17311,7 @@
         <v>13</v>
       </c>
       <c r="D411" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="E411" t="s">
         <v>661</v>
@@ -17363,7 +17363,7 @@
         <v>1</v>
       </c>
       <c r="D413" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="E413" t="s">
         <v>665</v>
@@ -17389,7 +17389,7 @@
         <v>2</v>
       </c>
       <c r="D414" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E414" t="s">
         <v>667</v>
@@ -17545,7 +17545,7 @@
         <v>5</v>
       </c>
       <c r="D420" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="E420" t="s">
         <v>676</v>
@@ -17597,7 +17597,7 @@
         <v>6</v>
       </c>
       <c r="D422" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="E422" t="s">
         <v>46</v>
@@ -17649,13 +17649,13 @@
         <v>7</v>
       </c>
       <c r="D424" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="E424" t="s">
         <v>230</v>
       </c>
       <c r="F424" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="G424">
         <v>1</v>
@@ -17701,7 +17701,7 @@
         <v>8</v>
       </c>
       <c r="D426" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="E426" t="s">
         <v>682</v>
@@ -17753,7 +17753,7 @@
         <v>1</v>
       </c>
       <c r="D428" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="E428" t="s">
         <v>686</v>
@@ -17779,7 +17779,7 @@
         <v>1</v>
       </c>
       <c r="D429" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="E429" t="s">
         <v>687</v>
@@ -17805,7 +17805,7 @@
         <v>2</v>
       </c>
       <c r="D430" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E430" t="s">
         <v>689</v>
@@ -17831,7 +17831,7 @@
         <v>2</v>
       </c>
       <c r="D431" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E431" t="s">
         <v>170</v>
@@ -17857,7 +17857,7 @@
         <v>3</v>
       </c>
       <c r="D432" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="E432" t="s">
         <v>157</v>
@@ -17909,7 +17909,7 @@
         <v>4</v>
       </c>
       <c r="D434" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="E434" t="s">
         <v>692</v>
@@ -17935,7 +17935,7 @@
         <v>4</v>
       </c>
       <c r="D435" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="E435" t="s">
         <v>17</v>
@@ -17987,7 +17987,7 @@
         <v>1</v>
       </c>
       <c r="D437" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="E437" t="s">
         <v>417</v>
@@ -18013,7 +18013,7 @@
         <v>2</v>
       </c>
       <c r="D438" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="E438" t="s">
         <v>699</v>
@@ -18039,7 +18039,7 @@
         <v>2</v>
       </c>
       <c r="D439" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="E439" t="s">
         <v>701</v>
@@ -18065,7 +18065,7 @@
         <v>3</v>
       </c>
       <c r="D440" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="E440" t="s">
         <v>703</v>
@@ -18091,7 +18091,7 @@
         <v>3</v>
       </c>
       <c r="D441" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="E441" t="s">
         <v>705</v>
@@ -18117,7 +18117,7 @@
         <v>4</v>
       </c>
       <c r="D442" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="E442" t="s">
         <v>631</v>
@@ -18169,7 +18169,7 @@
         <v>5</v>
       </c>
       <c r="D444" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="E444" t="s">
         <v>708</v>
@@ -18221,7 +18221,7 @@
         <v>6</v>
       </c>
       <c r="D446" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="E446" t="s">
         <v>711</v>
@@ -18247,7 +18247,7 @@
         <v>6</v>
       </c>
       <c r="D447" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="E447" t="s">
         <v>712</v>
@@ -18325,7 +18325,7 @@
         <v>8</v>
       </c>
       <c r="D450" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="E450" t="s">
         <v>268</v>
@@ -18351,7 +18351,7 @@
         <v>8</v>
       </c>
       <c r="D451" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="E451" t="s">
         <v>717</v>
@@ -18403,7 +18403,7 @@
         <v>1</v>
       </c>
       <c r="D453" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="E453" t="s">
         <v>532</v>
@@ -18429,7 +18429,7 @@
         <v>2</v>
       </c>
       <c r="D454" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="E454" t="s">
         <v>102</v>
@@ -18533,7 +18533,7 @@
         <v>2</v>
       </c>
       <c r="D458" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="E458" t="s">
         <v>730</v>
@@ -18559,7 +18559,7 @@
         <v>2</v>
       </c>
       <c r="D459" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="E459" t="s">
         <v>182</v>
@@ -18611,7 +18611,7 @@
         <v>3</v>
       </c>
       <c r="D461" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E461" t="s">
         <v>40</v>
@@ -18689,7 +18689,7 @@
         <v>2</v>
       </c>
       <c r="D464" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="E464" t="s">
         <v>119</v>
@@ -18715,7 +18715,7 @@
         <v>2</v>
       </c>
       <c r="D465" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E465" t="s">
         <v>486</v>
@@ -18793,7 +18793,7 @@
         <v>4</v>
       </c>
       <c r="D468" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="E468" t="s">
         <v>657</v>
@@ -18819,7 +18819,7 @@
         <v>4</v>
       </c>
       <c r="D469" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="E469" t="s">
         <v>711</v>
@@ -18897,7 +18897,7 @@
         <v>2</v>
       </c>
       <c r="D472" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="E472" t="s">
         <v>748</v>
@@ -18923,7 +18923,7 @@
         <v>2</v>
       </c>
       <c r="D473" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="E473" t="s">
         <v>408</v>
@@ -18949,7 +18949,7 @@
         <v>1</v>
       </c>
       <c r="D474" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="E474" t="s">
         <v>752</v>
@@ -18975,7 +18975,7 @@
         <v>1</v>
       </c>
       <c r="D475" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="E475" t="s">
         <v>754</v>
@@ -19001,7 +19001,7 @@
         <v>2</v>
       </c>
       <c r="D476" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="E476" t="s">
         <v>665</v>
@@ -19027,7 +19027,7 @@
         <v>2</v>
       </c>
       <c r="D477" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="E477" t="s">
         <v>641</v>
@@ -19053,7 +19053,7 @@
         <v>3</v>
       </c>
       <c r="D478" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="E478" t="s">
         <v>417</v>
@@ -19079,7 +19079,7 @@
         <v>3</v>
       </c>
       <c r="D479" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="E479" t="s">
         <v>408</v>
@@ -19105,7 +19105,7 @@
         <v>4</v>
       </c>
       <c r="D480" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="E480" t="s">
         <v>394</v>
@@ -19209,7 +19209,7 @@
         <v>6</v>
       </c>
       <c r="D484" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="E484" t="s">
         <v>492</v>
@@ -19235,7 +19235,7 @@
         <v>6</v>
       </c>
       <c r="D485" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="E485" t="s">
         <v>762</v>
@@ -19287,7 +19287,7 @@
         <v>7</v>
       </c>
       <c r="D487" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="E487" t="s">
         <v>451</v>
@@ -19313,7 +19313,7 @@
         <v>8</v>
       </c>
       <c r="D488" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="E488" t="s">
         <v>21</v>
@@ -19339,7 +19339,7 @@
         <v>8</v>
       </c>
       <c r="D489" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="E489" t="s">
         <v>766</v>
@@ -19365,7 +19365,7 @@
         <v>9</v>
       </c>
       <c r="D490" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="E490" t="s">
         <v>320</v>
@@ -19391,7 +19391,7 @@
         <v>9</v>
       </c>
       <c r="D491" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="E491" t="s">
         <v>769</v>
@@ -19417,7 +19417,7 @@
         <v>10</v>
       </c>
       <c r="D492" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="E492" t="s">
         <v>752</v>
@@ -19443,7 +19443,7 @@
         <v>10</v>
       </c>
       <c r="D493" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="E493" t="s">
         <v>40</v>
@@ -19469,7 +19469,7 @@
         <v>11</v>
       </c>
       <c r="D494" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="E494" t="s">
         <v>17</v>
@@ -19521,7 +19521,7 @@
         <v>12</v>
       </c>
       <c r="D496" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="E496" t="s">
         <v>775</v>
@@ -19573,7 +19573,7 @@
         <v>1</v>
       </c>
       <c r="D498" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="E498" t="s">
         <v>780</v>
@@ -19625,7 +19625,7 @@
         <v>2</v>
       </c>
       <c r="D500" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="E500" t="s">
         <v>783</v>
@@ -19755,7 +19755,7 @@
         <v>1</v>
       </c>
       <c r="D505" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="E505" t="s">
         <v>794</v>
@@ -19807,7 +19807,7 @@
         <v>2</v>
       </c>
       <c r="D507" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="E507" t="s">
         <v>797</v>
@@ -19859,7 +19859,7 @@
         <v>3</v>
       </c>
       <c r="D509" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="E509" t="s">
         <v>293</v>
@@ -19911,7 +19911,7 @@
         <v>4</v>
       </c>
       <c r="D511" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="E511" t="s">
         <v>803</v>
@@ -19937,7 +19937,7 @@
         <v>5</v>
       </c>
       <c r="D512" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="E512" t="s">
         <v>604</v>
@@ -20041,7 +20041,7 @@
         <v>7</v>
       </c>
       <c r="D516" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="E516" t="s">
         <v>809</v>
@@ -20067,7 +20067,7 @@
         <v>7</v>
       </c>
       <c r="D517" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E517" t="s">
         <v>60</v>
@@ -20119,7 +20119,7 @@
         <v>8</v>
       </c>
       <c r="D519" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="E519" t="s">
         <v>814</v>
@@ -20145,13 +20145,13 @@
         <v>9</v>
       </c>
       <c r="D520" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="E520" t="s">
         <v>783</v>
       </c>
       <c r="F520" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G520">
         <v>1</v>
@@ -20275,7 +20275,7 @@
         <v>12</v>
       </c>
       <c r="D525" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="E525" t="s">
         <v>822</v>
@@ -20301,7 +20301,7 @@
         <v>12</v>
       </c>
       <c r="D526" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="E526" t="s">
         <v>17</v>
@@ -20405,7 +20405,7 @@
         <v>15</v>
       </c>
       <c r="D530" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="E530" t="s">
         <v>831</v>
@@ -20431,7 +20431,7 @@
         <v>15</v>
       </c>
       <c r="D531" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="E531" t="s">
         <v>832</v>
@@ -20483,7 +20483,7 @@
         <v>16</v>
       </c>
       <c r="D533" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="E533" t="s">
         <v>836</v>
@@ -20509,7 +20509,7 @@
         <v>17</v>
       </c>
       <c r="D534" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="E534" t="s">
         <v>460</v>
@@ -20535,7 +20535,7 @@
         <v>17</v>
       </c>
       <c r="D535" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="E535" t="s">
         <v>157</v>
@@ -20561,7 +20561,7 @@
         <v>18</v>
       </c>
       <c r="D536" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="E536" t="s">
         <v>840</v>
@@ -20587,7 +20587,7 @@
         <v>18</v>
       </c>
       <c r="D537" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="E537" t="s">
         <v>841</v>
@@ -20639,7 +20639,7 @@
         <v>19</v>
       </c>
       <c r="D539" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="E539" t="s">
         <v>428</v>
@@ -20665,7 +20665,7 @@
         <v>20</v>
       </c>
       <c r="D540" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="E540" t="s">
         <v>70</v>
@@ -20691,7 +20691,7 @@
         <v>20</v>
       </c>
       <c r="D541" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="E541" t="s">
         <v>486</v>
@@ -20717,7 +20717,7 @@
         <v>21</v>
       </c>
       <c r="D542" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="E542" t="s">
         <v>847</v>
@@ -20795,7 +20795,7 @@
         <v>22</v>
       </c>
       <c r="D545" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="E545" t="s">
         <v>852</v>
@@ -20847,7 +20847,7 @@
         <v>23</v>
       </c>
       <c r="D547" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="E547" t="s">
         <v>794</v>
@@ -20899,7 +20899,7 @@
         <v>24</v>
       </c>
       <c r="D549" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="E549" t="s">
         <v>657</v>
@@ -20925,7 +20925,7 @@
         <v>25</v>
       </c>
       <c r="D550" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="E550" t="s">
         <v>437</v>
@@ -20951,7 +20951,7 @@
         <v>25</v>
       </c>
       <c r="D551" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="E551" t="s">
         <v>859</v>
@@ -21003,7 +21003,7 @@
         <v>26</v>
       </c>
       <c r="D553" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="E553" t="s">
         <v>657</v>
@@ -21029,7 +21029,7 @@
         <v>1</v>
       </c>
       <c r="D554" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="E554" t="s">
         <v>752</v>
@@ -21055,7 +21055,7 @@
         <v>1</v>
       </c>
       <c r="D555" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="E555" t="s">
         <v>863</v>
@@ -21133,7 +21133,7 @@
         <v>3</v>
       </c>
       <c r="D558" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="E558" t="s">
         <v>604</v>
@@ -21159,7 +21159,7 @@
         <v>3</v>
       </c>
       <c r="D559" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="E559" t="s">
         <v>124</v>
@@ -21211,7 +21211,7 @@
         <v>4</v>
       </c>
       <c r="D561" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="E561" t="s">
         <v>282</v>
@@ -21237,7 +21237,7 @@
         <v>5</v>
       </c>
       <c r="D562" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="E562" t="s">
         <v>871</v>
@@ -21263,7 +21263,7 @@
         <v>5</v>
       </c>
       <c r="D563" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="E563" t="s">
         <v>873</v>
@@ -21315,7 +21315,7 @@
         <v>6</v>
       </c>
       <c r="D565" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="E565" t="s">
         <v>406</v>
@@ -21341,7 +21341,7 @@
         <v>7</v>
       </c>
       <c r="D566" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="E566" t="s">
         <v>40</v>
@@ -21393,7 +21393,7 @@
         <v>8</v>
       </c>
       <c r="D568" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="E568" t="s">
         <v>367</v>
@@ -21445,7 +21445,7 @@
         <v>9</v>
       </c>
       <c r="D570" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="E570" t="s">
         <v>607</v>
@@ -21471,7 +21471,7 @@
         <v>9</v>
       </c>
       <c r="D571" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="E571" t="s">
         <v>881</v>
@@ -21497,7 +21497,7 @@
         <v>10</v>
       </c>
       <c r="D572" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="E572" t="s">
         <v>540</v>
@@ -21601,7 +21601,7 @@
         <v>12</v>
       </c>
       <c r="D576" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="E576" t="s">
         <v>889</v>
@@ -21679,7 +21679,7 @@
         <v>13</v>
       </c>
       <c r="D579" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="E579" t="s">
         <v>893</v>
@@ -21835,7 +21835,7 @@
         <v>2</v>
       </c>
       <c r="D585" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="E585" t="s">
         <v>167</v>
@@ -21913,7 +21913,7 @@
         <v>3</v>
       </c>
       <c r="D588" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E588" t="s">
         <v>125</v>
@@ -21939,7 +21939,7 @@
         <v>4</v>
       </c>
       <c r="D589" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="E589" t="s">
         <v>155</v>
@@ -21991,7 +21991,7 @@
         <v>5</v>
       </c>
       <c r="D591" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="E591" t="s">
         <v>408</v>
@@ -22017,7 +22017,7 @@
         <v>5</v>
       </c>
       <c r="D592" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="E592" t="s">
         <v>668</v>
@@ -22069,7 +22069,7 @@
         <v>6</v>
       </c>
       <c r="D594" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="E594" t="s">
         <v>233</v>
@@ -22225,7 +22225,7 @@
         <v>9</v>
       </c>
       <c r="D600" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="E600" t="s">
         <v>919</v>
@@ -22251,7 +22251,7 @@
         <v>10</v>
       </c>
       <c r="D601" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="E601" t="s">
         <v>157</v>
@@ -22303,7 +22303,7 @@
         <v>11</v>
       </c>
       <c r="D603" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="E603" t="s">
         <v>923</v>
@@ -22329,7 +22329,7 @@
         <v>11</v>
       </c>
       <c r="D604" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="E604" t="s">
         <v>131</v>
@@ -22355,7 +22355,7 @@
         <v>12</v>
       </c>
       <c r="D605" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="E605" t="s">
         <v>567</v>
@@ -22381,7 +22381,7 @@
         <v>12</v>
       </c>
       <c r="D606" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="E606" t="s">
         <v>926</v>
@@ -22433,7 +22433,7 @@
         <v>13</v>
       </c>
       <c r="D608" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E608" t="s">
         <v>930</v>
@@ -22459,7 +22459,7 @@
         <v>14</v>
       </c>
       <c r="D609" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="E609" t="s">
         <v>40</v>
@@ -22485,7 +22485,7 @@
         <v>14</v>
       </c>
       <c r="D610" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="E610" t="s">
         <v>102</v>
@@ -22511,13 +22511,13 @@
         <v>15</v>
       </c>
       <c r="D611" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="E611" t="s">
         <v>17</v>
       </c>
       <c r="F611" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="G611">
         <v>1</v>
@@ -22537,13 +22537,13 @@
         <v>15</v>
       </c>
       <c r="D612" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E612" t="s">
         <v>28</v>
       </c>
       <c r="F612" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="G612">
         <v>0</v>
@@ -22667,7 +22667,7 @@
         <v>3</v>
       </c>
       <c r="D617" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="E617" t="s">
         <v>492</v>
@@ -22693,7 +22693,7 @@
         <v>3</v>
       </c>
       <c r="D618" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="E618" t="s">
         <v>939</v>
@@ -22823,7 +22823,7 @@
         <v>1</v>
       </c>
       <c r="D623" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="E623" t="s">
         <v>947</v>
@@ -22849,7 +22849,7 @@
         <v>1</v>
       </c>
       <c r="D624" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="E624" t="s">
         <v>394</v>
@@ -22901,7 +22901,7 @@
         <v>2</v>
       </c>
       <c r="D626" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="E626" t="s">
         <v>437</v>
@@ -22979,7 +22979,7 @@
         <v>4</v>
       </c>
       <c r="D629" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="E629" t="s">
         <v>398</v>
@@ -23187,7 +23187,7 @@
         <v>2</v>
       </c>
       <c r="D637" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="E637" t="s">
         <v>965</v>
@@ -23213,7 +23213,7 @@
         <v>2</v>
       </c>
       <c r="D638" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="E638" t="s">
         <v>312</v>
@@ -23317,7 +23317,7 @@
         <v>5</v>
       </c>
       <c r="D642" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="E642" t="s">
         <v>35</v>
@@ -23473,7 +23473,7 @@
         <v>8</v>
       </c>
       <c r="D648" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="E648" t="s">
         <v>102</v>
@@ -23525,7 +23525,7 @@
         <v>9</v>
       </c>
       <c r="D650" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="E650" t="s">
         <v>367</v>
@@ -23603,7 +23603,7 @@
         <v>10</v>
       </c>
       <c r="D653" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="E653" t="s">
         <v>983</v>
@@ -23629,7 +23629,7 @@
         <v>11</v>
       </c>
       <c r="D654" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="E654" t="s">
         <v>985</v>
@@ -23655,7 +23655,7 @@
         <v>11</v>
       </c>
       <c r="D655" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="E655" t="s">
         <v>408</v>
@@ -23759,7 +23759,7 @@
         <v>14</v>
       </c>
       <c r="D659" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="E659" t="s">
         <v>975</v>
@@ -23785,7 +23785,7 @@
         <v>15</v>
       </c>
       <c r="D660" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="E660" t="s">
         <v>590</v>
@@ -23811,7 +23811,7 @@
         <v>15</v>
       </c>
       <c r="D661" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="E661" t="s">
         <v>157</v>
@@ -23837,7 +23837,7 @@
         <v>16</v>
       </c>
       <c r="D662" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="E662" t="s">
         <v>17</v>
@@ -23863,7 +23863,7 @@
         <v>16</v>
       </c>
       <c r="D663" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="E663" t="s">
         <v>367</v>
@@ -23941,7 +23941,7 @@
         <v>1</v>
       </c>
       <c r="D666" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="E666" t="s">
         <v>40</v>
@@ -23967,7 +23967,7 @@
         <v>1</v>
       </c>
       <c r="D667" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="E667" t="s">
         <v>168</v>
@@ -24071,7 +24071,7 @@
         <v>1</v>
       </c>
       <c r="D671" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="E671" t="s">
         <v>748</v>
@@ -24097,7 +24097,7 @@
         <v>2</v>
       </c>
       <c r="D672" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="E672" t="s">
         <v>204</v>
@@ -24123,7 +24123,7 @@
         <v>2</v>
       </c>
       <c r="D673" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="E673" t="s">
         <v>1003</v>
@@ -24149,7 +24149,7 @@
         <v>3</v>
       </c>
       <c r="D674" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="E674" t="s">
         <v>665</v>
@@ -24175,7 +24175,7 @@
         <v>4</v>
       </c>
       <c r="D675" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="E675" t="s">
         <v>1006</v>
@@ -24201,7 +24201,7 @@
         <v>5</v>
       </c>
       <c r="D676" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E676" t="s">
         <v>1008</v>
@@ -24227,7 +24227,7 @@
         <v>5</v>
       </c>
       <c r="D677" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="E677" t="s">
         <v>1009</v>
@@ -24253,7 +24253,7 @@
         <v>6</v>
       </c>
       <c r="D678" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="E678" t="s">
         <v>341</v>
@@ -24305,7 +24305,7 @@
         <v>7</v>
       </c>
       <c r="D680" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="E680" t="s">
         <v>1014</v>
@@ -24409,7 +24409,7 @@
         <v>1</v>
       </c>
       <c r="D684" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="E684" t="s">
         <v>1021</v>
@@ -24461,7 +24461,7 @@
         <v>2</v>
       </c>
       <c r="D686" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="E686" t="s">
         <v>119</v>
@@ -24487,7 +24487,7 @@
         <v>3</v>
       </c>
       <c r="D687" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="E687" t="s">
         <v>877</v>
@@ -24513,7 +24513,7 @@
         <v>3</v>
       </c>
       <c r="D688" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="E688" t="s">
         <v>1026</v>
@@ -24539,7 +24539,7 @@
         <v>4</v>
       </c>
       <c r="D689" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="E689" t="s">
         <v>239</v>
@@ -24565,7 +24565,7 @@
         <v>4</v>
       </c>
       <c r="D690" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="E690" t="s">
         <v>1028</v>
@@ -24643,7 +24643,7 @@
         <v>6</v>
       </c>
       <c r="D693" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="E693" t="s">
         <v>86</v>
@@ -24669,7 +24669,7 @@
         <v>6</v>
       </c>
       <c r="D694" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="E694" t="s">
         <v>1033</v>
@@ -24695,7 +24695,7 @@
         <v>7</v>
       </c>
       <c r="D695" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="E695" t="s">
         <v>119</v>
@@ -24721,7 +24721,7 @@
         <v>7</v>
       </c>
       <c r="D696" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="E696" t="s">
         <v>1034</v>
@@ -24799,7 +24799,7 @@
         <v>9</v>
       </c>
       <c r="D699" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="E699" t="s">
         <v>80</v>
@@ -24877,7 +24877,7 @@
         <v>1</v>
       </c>
       <c r="D702" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="E702" t="s">
         <v>1043</v>
@@ -24929,7 +24929,7 @@
         <v>2</v>
       </c>
       <c r="D704" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="E704" t="s">
         <v>450</v>
@@ -24955,7 +24955,7 @@
         <v>3</v>
       </c>
       <c r="D705" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="E705" t="s">
         <v>1047</v>
@@ -24981,7 +24981,7 @@
         <v>3</v>
       </c>
       <c r="D706" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="E706" t="s">
         <v>353</v>
@@ -25007,7 +25007,7 @@
         <v>4</v>
       </c>
       <c r="D707" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="E707" t="s">
         <v>840</v>
@@ -25033,7 +25033,7 @@
         <v>4</v>
       </c>
       <c r="D708" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="E708" t="s">
         <v>1051</v>
@@ -25085,7 +25085,7 @@
         <v>5</v>
       </c>
       <c r="D710" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E710" t="s">
         <v>1055</v>
@@ -25111,7 +25111,7 @@
         <v>6</v>
       </c>
       <c r="D711" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="E711" t="s">
         <v>615</v>
@@ -25137,7 +25137,7 @@
         <v>7</v>
       </c>
       <c r="D712" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E712" t="s">
         <v>1057</v>
@@ -25163,7 +25163,7 @@
         <v>7</v>
       </c>
       <c r="D713" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="E713" t="s">
         <v>692</v>
@@ -25215,7 +25215,7 @@
         <v>8</v>
       </c>
       <c r="D715" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="E715" t="s">
         <v>554</v>
@@ -25241,7 +25241,7 @@
         <v>9</v>
       </c>
       <c r="D716" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="E716" t="s">
         <v>1061</v>
@@ -25319,7 +25319,7 @@
         <v>10</v>
       </c>
       <c r="D719" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E719" t="s">
         <v>210</v>
@@ -25345,7 +25345,7 @@
         <v>11</v>
       </c>
       <c r="D720" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="E720" t="s">
         <v>1065</v>
@@ -25397,7 +25397,7 @@
         <v>12</v>
       </c>
       <c r="D722" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="E722" t="s">
         <v>1069</v>
@@ -25423,7 +25423,7 @@
         <v>13</v>
       </c>
       <c r="D723" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="E723" t="s">
         <v>1071</v>
@@ -25449,7 +25449,7 @@
         <v>13</v>
       </c>
       <c r="D724" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="E724" t="s">
         <v>1072</v>
@@ -25501,7 +25501,7 @@
         <v>14</v>
       </c>
       <c r="D726" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="E726" t="s">
         <v>1074</v>
@@ -25631,7 +25631,7 @@
         <v>17</v>
       </c>
       <c r="D731" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="E731" t="s">
         <v>147</v>
@@ -25657,7 +25657,7 @@
         <v>17</v>
       </c>
       <c r="D732" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E732" t="s">
         <v>1082</v>
@@ -25683,7 +25683,7 @@
         <v>18</v>
       </c>
       <c r="D733" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E733" t="s">
         <v>358</v>
@@ -25709,7 +25709,7 @@
         <v>18</v>
       </c>
       <c r="D734" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E734" t="s">
         <v>1085</v>
@@ -25735,7 +25735,7 @@
         <v>19</v>
       </c>
       <c r="D735" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="E735" t="s">
         <v>1087</v>
@@ -25787,7 +25787,7 @@
         <v>20</v>
       </c>
       <c r="D737" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="E737" t="s">
         <v>873</v>
@@ -25839,7 +25839,7 @@
         <v>21</v>
       </c>
       <c r="D739" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="E739" t="s">
         <v>855</v>
@@ -25891,7 +25891,7 @@
         <v>22</v>
       </c>
       <c r="D741" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="E741" t="s">
         <v>602</v>
@@ -25917,7 +25917,7 @@
         <v>23</v>
       </c>
       <c r="D742" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="E742" t="s">
         <v>182</v>
@@ -25969,7 +25969,7 @@
         <v>24</v>
       </c>
       <c r="D744" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="E744" t="s">
         <v>1098</v>
@@ -26021,7 +26021,7 @@
         <v>25</v>
       </c>
       <c r="D746" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="E746" t="s">
         <v>500</v>
@@ -26047,7 +26047,7 @@
         <v>26</v>
       </c>
       <c r="D747" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="E747" t="s">
         <v>157</v>
@@ -26099,7 +26099,7 @@
         <v>27</v>
       </c>
       <c r="D749" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E749" t="s">
         <v>1103</v>
@@ -26151,7 +26151,7 @@
         <v>28</v>
       </c>
       <c r="D751" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="E751" t="s">
         <v>1106</v>
@@ -26177,7 +26177,7 @@
         <v>29</v>
       </c>
       <c r="D752" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="E752" t="s">
         <v>1107</v>
@@ -26203,7 +26203,7 @@
         <v>29</v>
       </c>
       <c r="D753" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E753" t="s">
         <v>21</v>
@@ -26255,13 +26255,13 @@
         <v>30</v>
       </c>
       <c r="D755" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="E755" t="s">
         <v>341</v>
       </c>
       <c r="F755" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="G755">
         <v>0</v>
@@ -26281,7 +26281,7 @@
         <v>31</v>
       </c>
       <c r="D756" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="E756" t="s">
         <v>86</v>
@@ -26359,7 +26359,7 @@
         <v>33</v>
       </c>
       <c r="D759" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="E759" t="s">
         <v>1112</v>
@@ -26385,7 +26385,7 @@
         <v>33</v>
       </c>
       <c r="D760" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="E760" t="s">
         <v>540</v>
@@ -26411,7 +26411,7 @@
         <v>34</v>
       </c>
       <c r="D761" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E761" t="s">
         <v>1114</v>
@@ -26437,7 +26437,7 @@
         <v>34</v>
       </c>
       <c r="D762" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="E762" t="s">
         <v>1116</v>
@@ -26489,7 +26489,7 @@
         <v>35</v>
       </c>
       <c r="D764" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="E764" t="s">
         <v>367</v>
@@ -26541,7 +26541,7 @@
         <v>36</v>
       </c>
       <c r="D766" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="E766" t="s">
         <v>1121</v>
@@ -26593,7 +26593,7 @@
         <v>37</v>
       </c>
       <c r="D768" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E768" t="s">
         <v>1124</v>
@@ -26619,7 +26619,7 @@
         <v>38</v>
       </c>
       <c r="D769" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="E769" t="s">
         <v>1005</v>
@@ -26645,7 +26645,7 @@
         <v>38</v>
       </c>
       <c r="D770" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="E770" t="s">
         <v>1127</v>
@@ -26697,7 +26697,7 @@
         <v>1</v>
       </c>
       <c r="D772" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="E772" t="s">
         <v>23</v>
@@ -26879,7 +26879,7 @@
         <v>1</v>
       </c>
       <c r="D779" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="E779" t="s">
         <v>1138</v>
@@ -26931,7 +26931,7 @@
         <v>1</v>
       </c>
       <c r="D781" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="E781" t="s">
         <v>21</v>
@@ -26957,7 +26957,7 @@
         <v>1</v>
       </c>
       <c r="D782" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E782" t="s">
         <v>1144</v>
@@ -27035,7 +27035,7 @@
         <v>3</v>
       </c>
       <c r="D785" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E785" t="s">
         <v>21</v>
@@ -27061,7 +27061,7 @@
         <v>3</v>
       </c>
       <c r="D786" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="E786" t="s">
         <v>323</v>
@@ -27087,7 +27087,7 @@
         <v>4</v>
       </c>
       <c r="D787" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E787" t="s">
         <v>1149</v>
@@ -27113,7 +27113,7 @@
         <v>4</v>
       </c>
       <c r="D788" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="E788" t="s">
         <v>1062</v>
@@ -27139,7 +27139,7 @@
         <v>5</v>
       </c>
       <c r="D789" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="E789" t="s">
         <v>408</v>
@@ -27191,7 +27191,7 @@
         <v>6</v>
       </c>
       <c r="D791" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E791" t="s">
         <v>1154</v>
@@ -27295,7 +27295,7 @@
         <v>8</v>
       </c>
       <c r="D795" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E795" t="s">
         <v>752</v>
@@ -27347,7 +27347,7 @@
         <v>9</v>
       </c>
       <c r="D797" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="E797" t="s">
         <v>1163</v>
@@ -27451,7 +27451,7 @@
         <v>11</v>
       </c>
       <c r="D801" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="E801" t="s">
         <v>1170</v>
@@ -27503,7 +27503,7 @@
         <v>1</v>
       </c>
       <c r="D803" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="E803" t="s">
         <v>1174</v>
@@ -27633,7 +27633,7 @@
         <v>3</v>
       </c>
       <c r="D808" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="E808" t="s">
         <v>204</v>
@@ -27737,7 +27737,7 @@
         <v>5</v>
       </c>
       <c r="D812" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="E812" t="s">
         <v>1186</v>
@@ -27815,13 +27815,13 @@
         <v>7</v>
       </c>
       <c r="D815" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="E815" t="s">
         <v>1189</v>
       </c>
       <c r="F815" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="G815">
         <v>1</v>
@@ -27841,7 +27841,7 @@
         <v>7</v>
       </c>
       <c r="D816" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="E816" t="s">
         <v>949</v>
@@ -27867,7 +27867,7 @@
         <v>8</v>
       </c>
       <c r="D817" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="E817" t="s">
         <v>198</v>
@@ -27893,13 +27893,13 @@
         <v>8</v>
       </c>
       <c r="D818" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="E818" t="s">
         <v>102</v>
       </c>
       <c r="F818" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="G818">
         <v>0</v>
@@ -27945,7 +27945,7 @@
         <v>9</v>
       </c>
       <c r="D820" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="E820" t="s">
         <v>95</v>
@@ -27997,7 +27997,7 @@
         <v>10</v>
       </c>
       <c r="D822" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="E822" t="s">
         <v>353</v>
@@ -28023,7 +28023,7 @@
         <v>1</v>
       </c>
       <c r="D823" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="E823" t="s">
         <v>1198</v>
@@ -28049,7 +28049,7 @@
         <v>1</v>
       </c>
       <c r="D824" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="E824" t="s">
         <v>1199</v>
@@ -28075,7 +28075,7 @@
         <v>2</v>
       </c>
       <c r="D825" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="E825" t="s">
         <v>756</v>
@@ -28101,7 +28101,7 @@
         <v>2</v>
       </c>
       <c r="D826" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="E826" t="s">
         <v>12</v>
@@ -28127,7 +28127,7 @@
         <v>1</v>
       </c>
       <c r="D827" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="E827" t="s">
         <v>1204</v>
@@ -28257,7 +28257,7 @@
         <v>3</v>
       </c>
       <c r="D832" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="E832" t="s">
         <v>1210</v>
@@ -28283,7 +28283,7 @@
         <v>4</v>
       </c>
       <c r="D833" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="E833" t="s">
         <v>1212</v>
@@ -28309,7 +28309,7 @@
         <v>4</v>
       </c>
       <c r="D834" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="E834" t="s">
         <v>641</v>
@@ -28387,7 +28387,7 @@
         <v>6</v>
       </c>
       <c r="D837" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="E837" t="s">
         <v>590</v>
@@ -28465,7 +28465,7 @@
         <v>8</v>
       </c>
       <c r="D840" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E840" t="s">
         <v>17</v>
@@ -28491,13 +28491,13 @@
         <v>1</v>
       </c>
       <c r="D841" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="E841" t="s">
         <v>1036</v>
       </c>
       <c r="F841" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="G841">
         <v>0</v>

</xml_diff>